<commit_message>
Update System - SR
</commit_message>
<xml_diff>
--- a/website/static/service_record.xlsx
+++ b/website/static/service_record.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$71</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$23</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -722,22 +722,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -745,39 +778,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1150,10 +1150,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K1048380"/>
+  <dimension ref="A2:K1048397"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:K20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
@@ -1172,62 +1172,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="24">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
     </row>
     <row r="4" spans="1:11" ht="16.5">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="2"/>
@@ -1254,19 +1254,19 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="33">
-      <c r="A8" s="92" t="s">
+      <c r="A8" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
     </row>
     <row r="9" spans="1:11" ht="13.9" customHeight="1">
       <c r="A9" s="3"/>
@@ -1295,34 +1295,34 @@
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="88"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
     </row>
     <row r="12" spans="1:11" ht="19.899999999999999" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83" t="s">
+      <c r="C12" s="79"/>
+      <c r="D12" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83" t="s">
+      <c r="E12" s="79"/>
+      <c r="F12" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="83"/>
+      <c r="G12" s="79"/>
       <c r="H12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1332,18 +1332,18 @@
     </row>
     <row r="13" spans="1:11" ht="14.45" customHeight="1">
       <c r="A13" s="4"/>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="87" t="s">
+      <c r="C13" s="80"/>
+      <c r="D13" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87" t="s">
+      <c r="E13" s="81"/>
+      <c r="F13" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="87"/>
+      <c r="G13" s="81"/>
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -1364,17 +1364,17 @@
       <c r="A15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="82">
+      <c r="B15" s="85">
         <v>35761</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="83" t="s">
+      <c r="C15" s="85"/>
+      <c r="D15" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="84" t="s">
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="86" t="s">
         <v>16</v>
       </c>
       <c r="I15" s="13"/>
@@ -1383,17 +1383,17 @@
     </row>
     <row r="16" spans="1:11" ht="16.5">
       <c r="A16" s="12"/>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85" t="s">
+      <c r="C16" s="80"/>
+      <c r="D16" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="84"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="86"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
@@ -1406,48 +1406,48 @@
       <c r="E17" s="15"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="84"/>
+      <c r="H17" s="86"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="86"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="86"/>
-      <c r="J19" s="86"/>
-      <c r="K19" s="86"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="87"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="86"/>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="86"/>
-      <c r="J20" s="86"/>
-      <c r="K20" s="86"/>
+      <c r="A20" s="87"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="16"/>
@@ -1463,27 +1463,27 @@
       <c r="K21" s="16"/>
     </row>
     <row r="22" spans="1:11" s="17" customFormat="1" ht="30" customHeight="1">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="76"/>
-      <c r="C22" s="77" t="s">
+      <c r="B22" s="82"/>
+      <c r="C22" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="80" t="s">
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="76" t="s">
+      <c r="I22" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="77" t="s">
+      <c r="J22" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="79"/>
+      <c r="K22" s="84"/>
     </row>
     <row r="23" spans="1:11" s="17" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="18" t="s">
@@ -1492,19 +1492,19 @@
       <c r="B23" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="79"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="77" t="s">
+      <c r="F23" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="79"/>
-      <c r="H23" s="81"/>
-      <c r="I23" s="76"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="82"/>
       <c r="J23" s="20" t="s">
         <v>10</v>
       </c>
@@ -1733,381 +1733,595 @@
       <c r="J40" s="21"/>
       <c r="K40" s="26"/>
     </row>
-    <row r="41" spans="1:11" s="33" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="31"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="28"/>
       <c r="E41" s="22"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="32"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="25"/>
       <c r="I41" s="30"/>
       <c r="J41" s="21"/>
       <c r="K41" s="26"/>
     </row>
-    <row r="42" spans="1:11" ht="15" customHeight="1">
-      <c r="A42" s="37" t="s">
+    <row r="42" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="26"/>
+    </row>
+    <row r="43" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="26"/>
+    </row>
+    <row r="44" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="26"/>
+    </row>
+    <row r="45" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="26"/>
+    </row>
+    <row r="46" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="26"/>
+    </row>
+    <row r="47" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="26"/>
+    </row>
+    <row r="48" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="26"/>
+    </row>
+    <row r="49" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="26"/>
+    </row>
+    <row r="50" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="26"/>
+    </row>
+    <row r="51" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="26"/>
+    </row>
+    <row r="52" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="26"/>
+    </row>
+    <row r="53" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="26"/>
+    </row>
+    <row r="54" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="26"/>
+    </row>
+    <row r="55" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="26"/>
+    </row>
+    <row r="56" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A56" s="21"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="29"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="26"/>
+    </row>
+    <row r="57" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="30"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="26"/>
+    </row>
+    <row r="58" spans="1:11" s="33" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="30"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="26"/>
+    </row>
+    <row r="59" spans="1:11" ht="15" customHeight="1">
+      <c r="A59" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="40"/>
-    </row>
-    <row r="43" spans="1:11" ht="15" customHeight="1">
-      <c r="A43" s="41" t="s">
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="40"/>
+    </row>
+    <row r="60" spans="1:11" ht="15" customHeight="1">
+      <c r="A60" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-    </row>
-    <row r="44" spans="1:11" ht="15" customHeight="1">
-      <c r="A44" s="41"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
-      <c r="K44" s="42"/>
-    </row>
-    <row r="45" spans="1:11" ht="7.15" customHeight="1">
-      <c r="A45" s="41"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-    </row>
-    <row r="46" spans="1:11" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A46" s="44" t="s">
+      <c r="B60" s="42"/>
+      <c r="C60" s="42"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
+      <c r="H60" s="42"/>
+      <c r="I60" s="42"/>
+      <c r="J60" s="42"/>
+      <c r="K60" s="42"/>
+    </row>
+    <row r="61" spans="1:11" ht="15" customHeight="1">
+      <c r="A61" s="41"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="42"/>
+      <c r="I61" s="42"/>
+      <c r="J61" s="42"/>
+      <c r="K61" s="42"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="41"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="44"/>
+      <c r="I62" s="44"/>
+      <c r="J62" s="44"/>
+      <c r="K62" s="44"/>
+    </row>
+    <row r="63" spans="1:11" s="6" customFormat="1" ht="15" customHeight="1">
+      <c r="A63" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-    </row>
-    <row r="47" spans="1:11" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="44"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="50"/>
-      <c r="K47" s="50"/>
-    </row>
-    <row r="48" spans="1:11" ht="15" customHeight="1">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="39"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
-    </row>
-    <row r="49" spans="1:11" ht="15" customHeight="1">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="39"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="33"/>
-    </row>
-    <row r="50" spans="1:11" ht="15" customHeight="1">
-      <c r="A50" s="53"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="39"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="33"/>
-    </row>
-    <row r="51" spans="1:11" ht="5.0999999999999996" customHeight="1">
-      <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="39"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="52"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="33"/>
-    </row>
-    <row r="52" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A52" s="74" t="s">
+      <c r="B63" s="46"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="48"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="44"/>
+      <c r="I63" s="44"/>
+      <c r="J63" s="50"/>
+      <c r="K63" s="50"/>
+    </row>
+    <row r="64" spans="1:11" s="6" customFormat="1" ht="15" customHeight="1">
+      <c r="A64" s="44"/>
+      <c r="B64" s="46"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="44"/>
+      <c r="I64" s="44"/>
+      <c r="J64" s="50"/>
+      <c r="K64" s="50"/>
+    </row>
+    <row r="65" spans="1:11" ht="15" customHeight="1">
+      <c r="A65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="39"/>
+      <c r="F65" s="52"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="33"/>
+    </row>
+    <row r="66" spans="1:11" ht="15" customHeight="1">
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="39"/>
+      <c r="F66" s="52"/>
+      <c r="G66" s="52"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="33"/>
+      <c r="K66" s="33"/>
+    </row>
+    <row r="67" spans="1:11" ht="15" customHeight="1">
+      <c r="A67" s="53"/>
+      <c r="B67" s="53"/>
+      <c r="C67" s="53"/>
+      <c r="D67" s="39"/>
+      <c r="F67" s="52"/>
+      <c r="G67" s="52"/>
+      <c r="H67" s="53"/>
+      <c r="I67" s="53"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="33"/>
+    </row>
+    <row r="68" spans="1:11" ht="5.0999999999999996" customHeight="1">
+      <c r="A68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="39"/>
+      <c r="F68" s="52"/>
+      <c r="G68" s="52"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+      <c r="J68" s="33"/>
+      <c r="K68" s="33"/>
+    </row>
+    <row r="69" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A69" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="74"/>
-      <c r="C52" s="74"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="56"/>
-    </row>
-    <row r="53" spans="1:11" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A53" s="75" t="s">
+      <c r="B69" s="88"/>
+      <c r="C69" s="88"/>
+      <c r="D69" s="88"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
+      <c r="H69" s="56"/>
+      <c r="I69" s="56"/>
+      <c r="J69" s="56"/>
+      <c r="K69" s="56"/>
+    </row>
+    <row r="70" spans="1:11" s="6" customFormat="1" ht="15" customHeight="1">
+      <c r="A70" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="B53" s="75"/>
-      <c r="C53" s="75"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="57"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="58"/>
-      <c r="K53" s="58"/>
-    </row>
-    <row r="54" spans="1:11" ht="9.9499999999999993" customHeight="1">
-      <c r="A54" s="39"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="59"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="52"/>
-      <c r="I54" s="33"/>
-      <c r="J54" s="33"/>
-      <c r="K54" s="33"/>
-    </row>
-    <row r="55" spans="1:11" ht="15" customHeight="1">
-      <c r="A55" s="39"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="60"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="52"/>
-      <c r="I55" s="33"/>
-      <c r="J55" s="33"/>
-      <c r="K55" s="33"/>
-    </row>
-    <row r="56" spans="1:11" ht="12" customHeight="1">
-      <c r="A56" s="61"/>
-      <c r="B56" s="62"/>
-      <c r="C56" s="63"/>
-      <c r="D56" s="64"/>
-      <c r="E56" s="65"/>
-      <c r="F56" s="66"/>
-      <c r="G56" s="66"/>
-      <c r="H56" s="64"/>
-      <c r="I56" s="67"/>
-      <c r="J56" s="67"/>
-      <c r="K56" s="67"/>
-    </row>
-    <row r="57" spans="1:11" ht="12" customHeight="1">
-      <c r="A57" s="68"/>
-      <c r="B57" s="69"/>
-      <c r="C57" s="69"/>
-      <c r="D57" s="64"/>
-      <c r="E57" s="65"/>
-      <c r="F57" s="66"/>
-      <c r="G57" s="66"/>
-      <c r="H57" s="64"/>
-      <c r="I57" s="67"/>
-      <c r="J57" s="67"/>
-      <c r="K57" s="67"/>
-    </row>
-    <row r="58" spans="1:11" ht="12" customHeight="1">
-      <c r="A58" s="70"/>
-      <c r="B58" s="62"/>
-      <c r="C58" s="63"/>
-      <c r="D58" s="64"/>
-      <c r="E58" s="65"/>
-      <c r="F58" s="66"/>
-      <c r="G58" s="66"/>
-      <c r="H58" s="64"/>
-      <c r="I58" s="64"/>
-      <c r="J58" s="64"/>
-      <c r="K58" s="64"/>
-    </row>
-    <row r="59" spans="1:11" ht="12" customHeight="1">
-      <c r="A59" s="70"/>
-      <c r="B59" s="62"/>
-      <c r="C59" s="71"/>
-      <c r="D59" s="64"/>
-      <c r="E59" s="65"/>
-      <c r="F59" s="64"/>
-      <c r="G59" s="64"/>
-      <c r="H59" s="64"/>
-      <c r="I59" s="64"/>
-      <c r="J59" s="64"/>
-      <c r="K59" s="64"/>
-    </row>
-    <row r="60" spans="1:11" ht="15">
-      <c r="A60" s="72"/>
-      <c r="B60" s="62"/>
-      <c r="C60" s="63"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="65"/>
-      <c r="F60" s="64"/>
-      <c r="G60" s="64"/>
-      <c r="H60" s="64"/>
-      <c r="I60" s="64"/>
-      <c r="J60" s="64"/>
-      <c r="K60" s="64"/>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" s="64"/>
-      <c r="B61" s="64"/>
-      <c r="C61" s="71"/>
-      <c r="D61" s="64"/>
-      <c r="E61" s="65"/>
-      <c r="F61" s="64"/>
-      <c r="G61" s="64"/>
-      <c r="H61" s="64"/>
-      <c r="I61" s="64"/>
-      <c r="J61" s="64"/>
-      <c r="K61" s="64"/>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="64"/>
-      <c r="B62" s="64"/>
-      <c r="C62" s="71"/>
-      <c r="D62" s="64"/>
-      <c r="E62" s="65"/>
-      <c r="F62" s="64"/>
-      <c r="G62" s="64"/>
-      <c r="H62" s="64"/>
-      <c r="I62" s="64"/>
-      <c r="J62" s="64"/>
-      <c r="K62" s="64"/>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="64"/>
-      <c r="B63" s="64"/>
-      <c r="C63" s="71"/>
-      <c r="D63" s="64"/>
-      <c r="E63" s="65"/>
-      <c r="F63" s="64"/>
-      <c r="G63" s="64"/>
-      <c r="H63" s="64"/>
-      <c r="I63" s="64"/>
-      <c r="J63" s="64"/>
-      <c r="K63" s="64"/>
-    </row>
-    <row r="64" spans="1:11">
-      <c r="A64" s="64"/>
-      <c r="B64" s="64"/>
-      <c r="C64" s="71"/>
-      <c r="D64" s="64"/>
-      <c r="E64" s="65"/>
-      <c r="F64" s="64"/>
-      <c r="G64" s="64"/>
-      <c r="H64" s="64"/>
-      <c r="I64" s="64"/>
-      <c r="J64" s="64"/>
-      <c r="K64" s="64"/>
-    </row>
-    <row r="65" spans="1:11">
-      <c r="A65" s="64"/>
-      <c r="B65" s="64"/>
-      <c r="C65" s="71"/>
-      <c r="D65" s="64"/>
-      <c r="E65" s="65"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="64"/>
-      <c r="H65" s="64"/>
-      <c r="I65" s="64"/>
-      <c r="J65" s="64"/>
-      <c r="K65" s="64"/>
-    </row>
-    <row r="66" spans="1:11">
-      <c r="A66" s="64"/>
-      <c r="B66" s="64"/>
-      <c r="C66" s="71"/>
-      <c r="D66" s="64"/>
-      <c r="E66" s="65"/>
-      <c r="F66" s="64"/>
-      <c r="G66" s="64"/>
-      <c r="H66" s="64"/>
-      <c r="I66" s="64"/>
-      <c r="J66" s="64"/>
-      <c r="K66" s="64"/>
-    </row>
-    <row r="67" spans="1:11">
-      <c r="C67" s="59"/>
-    </row>
-    <row r="68" spans="1:11">
-      <c r="C68" s="59"/>
-    </row>
-    <row r="69" spans="1:11">
-      <c r="C69" s="59"/>
-    </row>
-    <row r="70" spans="1:11">
-      <c r="C70" s="59"/>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="B70" s="89"/>
+      <c r="C70" s="89"/>
+      <c r="D70" s="89"/>
+      <c r="E70" s="48"/>
+      <c r="F70" s="57"/>
+      <c r="G70" s="57"/>
+      <c r="H70" s="58"/>
+      <c r="I70" s="58"/>
+      <c r="J70" s="58"/>
+      <c r="K70" s="58"/>
+    </row>
+    <row r="71" spans="1:11" ht="9.9499999999999993" customHeight="1">
+      <c r="A71" s="39"/>
+      <c r="B71" s="43"/>
       <c r="C71" s="59"/>
-    </row>
-    <row r="72" spans="1:11">
-      <c r="C72" s="59"/>
-    </row>
-    <row r="1048380" spans="5:5">
-      <c r="E1048380" s="73" t="s">
+      <c r="F71" s="52"/>
+      <c r="G71" s="52"/>
+      <c r="I71" s="33"/>
+      <c r="J71" s="33"/>
+      <c r="K71" s="33"/>
+    </row>
+    <row r="72" spans="1:11" ht="15" customHeight="1">
+      <c r="A72" s="39"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="60"/>
+      <c r="F72" s="52"/>
+      <c r="G72" s="52"/>
+      <c r="I72" s="33"/>
+      <c r="J72" s="33"/>
+      <c r="K72" s="33"/>
+    </row>
+    <row r="73" spans="1:11" ht="12" customHeight="1">
+      <c r="A73" s="61"/>
+      <c r="B73" s="62"/>
+      <c r="C73" s="63"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="65"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="64"/>
+      <c r="I73" s="67"/>
+      <c r="J73" s="67"/>
+      <c r="K73" s="67"/>
+    </row>
+    <row r="74" spans="1:11" ht="12" customHeight="1">
+      <c r="A74" s="68"/>
+      <c r="B74" s="69"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="65"/>
+      <c r="F74" s="66"/>
+      <c r="G74" s="66"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="67"/>
+      <c r="J74" s="67"/>
+      <c r="K74" s="67"/>
+    </row>
+    <row r="75" spans="1:11" ht="12" customHeight="1">
+      <c r="A75" s="70"/>
+      <c r="B75" s="62"/>
+      <c r="C75" s="63"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="65"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="66"/>
+      <c r="H75" s="64"/>
+      <c r="I75" s="64"/>
+      <c r="J75" s="64"/>
+      <c r="K75" s="64"/>
+    </row>
+    <row r="76" spans="1:11" ht="12" customHeight="1">
+      <c r="A76" s="70"/>
+      <c r="B76" s="62"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="65"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="64"/>
+      <c r="H76" s="64"/>
+      <c r="I76" s="64"/>
+      <c r="J76" s="64"/>
+      <c r="K76" s="64"/>
+    </row>
+    <row r="77" spans="1:11" ht="15">
+      <c r="A77" s="72"/>
+      <c r="B77" s="62"/>
+      <c r="C77" s="63"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="65"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="64"/>
+      <c r="H77" s="64"/>
+      <c r="I77" s="64"/>
+      <c r="J77" s="64"/>
+      <c r="K77" s="64"/>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="64"/>
+      <c r="B78" s="64"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="65"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="64"/>
+      <c r="H78" s="64"/>
+      <c r="I78" s="64"/>
+      <c r="J78" s="64"/>
+      <c r="K78" s="64"/>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="64"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="71"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="65"/>
+      <c r="F79" s="64"/>
+      <c r="G79" s="64"/>
+      <c r="H79" s="64"/>
+      <c r="I79" s="64"/>
+      <c r="J79" s="64"/>
+      <c r="K79" s="64"/>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="64"/>
+      <c r="B80" s="64"/>
+      <c r="C80" s="71"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="65"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="64"/>
+      <c r="H80" s="64"/>
+      <c r="I80" s="64"/>
+      <c r="J80" s="64"/>
+      <c r="K80" s="64"/>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" s="64"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="65"/>
+      <c r="F81" s="64"/>
+      <c r="G81" s="64"/>
+      <c r="H81" s="64"/>
+      <c r="I81" s="64"/>
+      <c r="J81" s="64"/>
+      <c r="K81" s="64"/>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="64"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="64"/>
+      <c r="E82" s="65"/>
+      <c r="F82" s="64"/>
+      <c r="G82" s="64"/>
+      <c r="H82" s="64"/>
+      <c r="I82" s="64"/>
+      <c r="J82" s="64"/>
+      <c r="K82" s="64"/>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" s="64"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="71"/>
+      <c r="D83" s="64"/>
+      <c r="E83" s="65"/>
+      <c r="F83" s="64"/>
+      <c r="G83" s="64"/>
+      <c r="H83" s="64"/>
+      <c r="I83" s="64"/>
+      <c r="J83" s="64"/>
+      <c r="K83" s="64"/>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="C84" s="59"/>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="C85" s="59"/>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="C86" s="59"/>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="C87" s="59"/>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="C88" s="59"/>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="C89" s="59"/>
+    </row>
+    <row r="1048397" spans="5:5">
+      <c r="E1048397" s="73" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:H23"/>
     <mergeCell ref="I22:I23"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="C23:D23"/>
@@ -2118,11 +2332,18 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:G16"/>
     <mergeCell ref="A18:K20"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A8:K8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.39370078740157499" bottom="0" header="0.25" footer="0"/>

</xml_diff>